<commit_message>
adding InitializingLayer state, that increments layer, displays print status, and goes to next state needed
</commit_message>
<xml_diff>
--- a/docs/Ember states and sub-states.xlsx
+++ b/docs/Ember states and sub-states.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="115">
   <si>
     <t>State</t>
   </si>
@@ -365,6 +365,12 @@
   <si>
     <t>Print data not found
 Place a single print file in the &lt;folder name&gt; folder of your drive.</t>
+  </si>
+  <si>
+    <t>InitializingLayer</t>
+  </si>
+  <si>
+    <t>Seaparating</t>
   </si>
 </sst>
 </file>
@@ -498,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -542,8 +548,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -634,29 +646,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -678,6 +693,9 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -699,6 +717,9 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -998,9 +1019,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="G20:H21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -1038,7 +1061,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1059,7 +1082,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="37"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1076,7 +1099,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="37"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="13" t="s">
         <v>62</v>
       </c>
@@ -1094,7 +1117,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="37"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="17" t="s">
         <v>64</v>
       </c>
@@ -1111,7 +1134,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="37"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="13" t="s">
         <v>56</v>
       </c>
@@ -1128,7 +1151,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="28">
-      <c r="A7" s="37"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1149,7 +1172,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="37"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1193,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="37"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="13" t="s">
         <v>58</v>
       </c>
@@ -1189,7 +1212,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="37"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="13" t="s">
         <v>71</v>
       </c>
@@ -1208,7 +1231,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="37"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="13" t="s">
         <v>72</v>
       </c>
@@ -1227,7 +1250,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="37"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="13" t="s">
         <v>73</v>
       </c>
@@ -1246,7 +1269,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="37"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="13" t="s">
         <v>109</v>
       </c>
@@ -1267,7 +1290,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="28">
-      <c r="A14" s="38"/>
+      <c r="A14" s="42"/>
       <c r="B14" t="s">
         <v>110</v>
       </c>
@@ -1286,7 +1309,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="13"/>
@@ -1303,7 +1326,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="38"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="13" t="s">
         <v>93</v>
       </c>
@@ -1326,13 +1349,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="37" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="17" t="s">
@@ -1344,12 +1367,12 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="29" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="G18" s="17" t="s">
         <v>83</v>
       </c>
@@ -1358,17 +1381,17 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="18" t="s">
-        <v>12</v>
+      <c r="A19" s="36" t="s">
+        <v>113</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
       <c r="G19" s="17" t="s">
         <v>80</v>
       </c>
@@ -1377,15 +1400,15 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="33" t="s">
-        <v>99</v>
+      <c r="A20" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
       <c r="G20" s="17" t="s">
         <v>80</v>
       </c>
@@ -1394,15 +1417,15 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="31" t="s">
-        <v>100</v>
+      <c r="A21" s="33" t="s">
+        <v>99</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="G21" s="17" t="s">
         <v>80</v>
       </c>
@@ -1412,14 +1435,14 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
       <c r="G22" s="17" t="s">
         <v>80</v>
       </c>
@@ -1428,15 +1451,15 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="34" t="s">
-        <v>102</v>
+      <c r="A23" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
       <c r="G23" s="17" t="s">
         <v>80</v>
       </c>
@@ -1445,15 +1468,15 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="27" t="s">
-        <v>92</v>
+      <c r="A24" s="34" t="s">
+        <v>102</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
       <c r="G24" s="17" t="s">
         <v>80</v>
       </c>
@@ -1462,15 +1485,15 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="18" t="s">
-        <v>8</v>
+      <c r="A25" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="G25" s="17" t="s">
         <v>80</v>
       </c>
@@ -1480,123 +1503,123 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="G26" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="G26" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="20" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="G27" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G28" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H28" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="19" t="s">
+    <row r="29" spans="1:8">
+      <c r="A29" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="7"/>
-      <c r="G28" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="18" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="7"/>
+      <c r="G29" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="32" t="s">
-        <v>104</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>95</v>
+        <v>45</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="25" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="36" t="s">
-        <v>15</v>
+      <c r="A31" s="32" t="s">
+        <v>104</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="7"/>
-      <c r="G31" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H31" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="37"/>
-      <c r="B32" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>60</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="7"/>
@@ -1604,16 +1627,16 @@
         <v>80</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="38"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="7"/>
@@ -1621,209 +1644,215 @@
         <v>80</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="28">
-      <c r="A34" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14" t="s">
-        <v>48</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="42"/>
+      <c r="B34" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="7"/>
       <c r="G34" s="17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="38"/>
-      <c r="B35" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>22</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28">
+      <c r="A35" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="7"/>
       <c r="G35" s="17" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H35" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28">
-      <c r="A36" s="18" t="s">
+    <row r="36" spans="1:8">
+      <c r="A36" s="42"/>
+      <c r="B36" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="7"/>
+      <c r="G36" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28">
+      <c r="A37" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14" t="s">
+      <c r="B37" s="13"/>
+      <c r="C37" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G37" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H37" s="25" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" s="25" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="13"/>
-      <c r="C38" s="14" t="s">
-        <v>59</v>
+      <c r="C38" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="28">
+      <c r="H38" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="G39" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H39" s="25" t="s">
-        <v>87</v>
+      <c r="H39" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28">
-      <c r="A40" s="31" t="s">
-        <v>98</v>
+      <c r="A40" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="7"/>
       <c r="G40" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="17" customFormat="1" ht="28">
-      <c r="A41" s="26" t="s">
-        <v>77</v>
+      <c r="H40" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28">
+      <c r="A41" s="31" t="s">
+        <v>98</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="22" t="s">
-        <v>43</v>
-      </c>
+      <c r="E41" s="30"/>
+      <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="17" customFormat="1" ht="28">
-      <c r="A42" s="35" t="s">
-        <v>107</v>
+      <c r="A42" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="17" customFormat="1" ht="28">
+      <c r="A43" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
-      <c r="G42" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="D43" s="21"/>
+      <c r="E43" s="22"/>
+      <c r="G43" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="8"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-    </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="8"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>87</v>
-      </c>
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>80</v>
@@ -1834,42 +1863,41 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="G47" t="s">
-        <v>81</v>
-      </c>
-      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H47" s="17" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G48" t="s">
-        <v>80</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="H48" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
         <v>8</v>
       </c>
-      <c r="G49" t="s">
-        <v>83</v>
-      </c>
-      <c r="H49" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" s="15"/>
       <c r="G50" t="s">
         <v>83</v>
       </c>
@@ -1879,7 +1907,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="17" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B51" s="15"/>
       <c r="G51" t="s">
@@ -1891,7 +1919,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" s="15"/>
       <c r="G52" t="s">
@@ -1903,7 +1931,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="17" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B53" s="15"/>
       <c r="G53" t="s">
@@ -1915,7 +1943,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B54" s="15"/>
       <c r="G54" t="s">
@@ -1927,27 +1955,51 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="G55" t="s">
+        <v>83</v>
+      </c>
+      <c r="H55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="G56" t="s">
+        <v>83</v>
+      </c>
+      <c r="H56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="G55" t="s">
-        <v>80</v>
-      </c>
-      <c r="H55" t="s">
+      <c r="G57" t="s">
+        <v>80</v>
+      </c>
+      <c r="H57" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="A34:A35"/>
     <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A32:A34"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C27"/>
+    <mergeCell ref="D19:D27"/>
+    <mergeCell ref="E19:E27"/>
+    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updating table of states and substates for new substates when door is open, and making Spark 'ready' status more explicit in some of those cases
</commit_message>
<xml_diff>
--- a/docs/Ember states and sub-states.xlsx
+++ b/docs/Ember states and sub-states.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="100" yWindow="400" windowWidth="17920" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="115">
   <si>
     <t>State</t>
   </si>
@@ -280,9 +280,6 @@
     <t>paused</t>
   </si>
   <si>
-    <t>maintenance</t>
-  </si>
-  <si>
     <t>error</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>Seaparating</t>
+  </si>
+  <si>
+    <t>maintenance (or ready, if Sark Printer Status was ready when the door was opened)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -554,8 +554,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -649,6 +661,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,17 +682,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -696,6 +712,12 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -720,6 +742,12 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1019,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="G20:H21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1057,11 +1085,11 @@
         <v>79</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1078,11 +1106,11 @@
         <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="43"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1099,7 +1127,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="43"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="13" t="s">
         <v>62</v>
       </c>
@@ -1117,7 +1145,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="43"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="17" t="s">
         <v>64</v>
       </c>
@@ -1130,11 +1158,11 @@
         <v>81</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="43"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="13" t="s">
         <v>56</v>
       </c>
@@ -1151,7 +1179,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="28">
-      <c r="A7" s="43"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1168,11 +1196,11 @@
         <v>81</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="43"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1189,11 +1217,11 @@
         <v>81</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="43"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="13" t="s">
         <v>58</v>
       </c>
@@ -1208,11 +1236,11 @@
         <v>81</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="43"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="13" t="s">
         <v>71</v>
       </c>
@@ -1227,11 +1255,11 @@
         <v>80</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="43"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="13" t="s">
         <v>72</v>
       </c>
@@ -1246,11 +1274,11 @@
         <v>81</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="43"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="13" t="s">
         <v>73</v>
       </c>
@@ -1265,37 +1293,37 @@
         <v>81</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="43"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28">
+      <c r="A14" s="39"/>
+      <c r="B14" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28">
-      <c r="A14" s="42"/>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>112</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22" t="s">
@@ -1305,11 +1333,11 @@
         <v>80</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="13"/>
@@ -1326,16 +1354,16 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="42"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>94</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>83</v>
@@ -1349,13 +1377,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="40" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="17" t="s">
@@ -1367,12 +1395,12 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
       <c r="G18" s="17" t="s">
         <v>83</v>
       </c>
@@ -1382,16 +1410,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
       <c r="G19" s="17" t="s">
         <v>80</v>
       </c>
@@ -1406,9 +1434,9 @@
       <c r="B20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="G20" s="17" t="s">
         <v>80</v>
       </c>
@@ -1418,14 +1446,14 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="G21" s="17" t="s">
         <v>80</v>
       </c>
@@ -1435,14 +1463,14 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
       <c r="G22" s="17" t="s">
         <v>80</v>
       </c>
@@ -1452,14 +1480,14 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="G23" s="17" t="s">
         <v>80</v>
       </c>
@@ -1469,14 +1497,14 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="G24" s="17" t="s">
         <v>80</v>
       </c>
@@ -1486,14 +1514,14 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="G25" s="17" t="s">
         <v>80</v>
       </c>
@@ -1508,9 +1536,9 @@
       <c r="B26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="G26" s="17" t="s">
         <v>80</v>
       </c>
@@ -1523,9 +1551,9 @@
         <v>67</v>
       </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="G27" s="17" t="s">
         <v>80</v>
       </c>
@@ -1594,27 +1622,27 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>80</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="13"/>
@@ -1627,11 +1655,11 @@
         <v>80</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="43"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="13" t="s">
         <v>16</v>
       </c>
@@ -1644,11 +1672,11 @@
         <v>80</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="42"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="13" t="s">
         <v>19</v>
       </c>
@@ -1661,11 +1689,11 @@
         <v>80</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="28">
-      <c r="A35" s="41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="70">
+      <c r="A35" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="13"/>
@@ -1674,15 +1702,15 @@
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="17" t="s">
-        <v>85</v>
+      <c r="G35" s="45" t="s">
+        <v>114</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="42"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="13" t="s">
         <v>21</v>
       </c>
@@ -1695,269 +1723,284 @@
         <v>80</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="28">
-      <c r="A37" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>5</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="38"/>
+      <c r="B37" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="7"/>
       <c r="G37" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="25" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="A38" s="38"/>
+      <c r="B38" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="14"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="E38" s="7"/>
       <c r="G38" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="25" t="s">
-        <v>87</v>
+      <c r="H38" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="14" t="s">
-        <v>59</v>
-      </c>
+      <c r="A39" s="38"/>
+      <c r="B39" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="14"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="E39" s="7"/>
       <c r="G39" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="28">
-      <c r="A40" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="H39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="38"/>
+      <c r="B40" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="4"/>
       <c r="E40" s="7"/>
       <c r="G40" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="28">
-      <c r="A41" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="17"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="39"/>
+      <c r="B41" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="44"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="7"/>
       <c r="G41" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="17" customFormat="1" ht="28">
-      <c r="A42" s="26" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28">
+      <c r="A42" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="28">
+      <c r="A45" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="G45" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28">
+      <c r="A46" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="30"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="17" customFormat="1" ht="28">
+      <c r="A47" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D47" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E47" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G42" s="17" t="s">
+      <c r="G47" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H47" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="17" customFormat="1" ht="28">
-      <c r="A43" s="35" t="s">
+    <row r="48" spans="1:8" s="17" customFormat="1" ht="28">
+      <c r="A48" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="22"/>
-      <c r="G43" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="D48" s="21"/>
+      <c r="E48" s="22"/>
+      <c r="G48" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="8"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1" t="s">
+    <row r="49" spans="1:8">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="8"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
+      <c r="G51" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="s">
+      <c r="G52" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H52" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G53" t="s">
         <v>81</v>
       </c>
-      <c r="H48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" t="s">
+      <c r="H53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
         <v>7</v>
       </c>
-      <c r="G49" t="s">
-        <v>80</v>
-      </c>
-      <c r="H49" s="24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" t="s">
+      <c r="G54" t="s">
+        <v>80</v>
+      </c>
+      <c r="H54" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
         <v>8</v>
       </c>
-      <c r="G50" t="s">
-        <v>83</v>
-      </c>
-      <c r="H50" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B51" s="15"/>
-      <c r="G51" t="s">
-        <v>83</v>
-      </c>
-      <c r="H51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="15"/>
-      <c r="G52" t="s">
-        <v>83</v>
-      </c>
-      <c r="H52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" s="15"/>
-      <c r="G53" t="s">
-        <v>83</v>
-      </c>
-      <c r="H53" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="15"/>
-      <c r="G54" t="s">
-        <v>83</v>
-      </c>
-      <c r="H54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="15"/>
       <c r="G55" t="s">
         <v>83</v>
       </c>
@@ -1967,7 +2010,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="17" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B56" s="15"/>
       <c r="G56" t="s">
@@ -1979,27 +2022,87 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="17" t="s">
-        <v>103</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B57" s="15"/>
       <c r="G57" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H57" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="G58" t="s">
+        <v>83</v>
+      </c>
+      <c r="H58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="G59" t="s">
+        <v>83</v>
+      </c>
+      <c r="H59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="15"/>
+      <c r="G60" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="15"/>
+      <c r="G61" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" t="s">
+        <v>80</v>
+      </c>
+      <c r="H62" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C27"/>
+    <mergeCell ref="D19:D27"/>
+    <mergeCell ref="E19:E27"/>
+    <mergeCell ref="A35:A41"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C27"/>
-    <mergeCell ref="D19:D27"/>
-    <mergeCell ref="E19:E27"/>
-    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updated description of error screen
</commit_message>
<xml_diff>
--- a/docs/Ember states and sub-states.xlsx
+++ b/docs/Ember states and sub-states.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="115">
   <si>
     <t>State</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Door open.  Please close the door ASAP to avoid exposing the photosensitive resin.</t>
   </si>
   <si>
-    <t>Error &lt;Ember error code&gt;:&lt;Linux errno&gt; &lt;short error message&gt; Return home or reset?</t>
-  </si>
-  <si>
     <t>Reset</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>Seaparating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error &lt;Ember error code&gt;:&lt;Linux errno&gt; &lt;short error message&gt; </t>
   </si>
 </sst>
 </file>
@@ -649,6 +649,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,15 +668,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="G20:H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>11</v>
@@ -1054,35 +1054,35 @@
         <v>2</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="43"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1092,51 +1092,51 @@
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
       <c r="G3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
         <v>81</v>
       </c>
-      <c r="H3" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="43"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="7"/>
       <c r="F4" s="16"/>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="43"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="43"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>36</v>
@@ -1144,16 +1144,16 @@
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28">
-      <c r="A7" s="43"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>31</v>
@@ -1165,14 +1165,14 @@
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="43"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1186,16 +1186,16 @@
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="43"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>34</v>
@@ -1205,111 +1205,111 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="43"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="43"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="43"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="43"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28">
+      <c r="A14" s="39"/>
+      <c r="B14" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28">
-      <c r="A14" s="42"/>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>112</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="13"/>
@@ -1319,29 +1319,29 @@
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="G15" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="42"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>94</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1349,54 +1349,54 @@
         <v>10</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="40" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
       <c r="G18" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
       <c r="G19" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1404,101 +1404,101 @@
         <v>12</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="G20" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="G21" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
       <c r="G22" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="G23" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="G24" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="G25" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1506,31 +1506,31 @@
         <v>8</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="G26" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="G27" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1548,27 +1548,27 @@
         <v>43</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="7"/>
       <c r="G29" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1586,86 +1586,86 @@
         <v>47</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="7"/>
       <c r="G32" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="43"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="7"/>
       <c r="G33" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="42"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="7"/>
       <c r="G34" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="13"/>
@@ -1675,14 +1675,14 @@
       <c r="D35" s="4"/>
       <c r="E35" s="7"/>
       <c r="G35" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="42"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="13" t="s">
         <v>21</v>
       </c>
@@ -1692,31 +1692,29 @@
       <c r="D36" s="4"/>
       <c r="E36" s="7"/>
       <c r="G36" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="E37" s="7"/>
       <c r="G37" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H37" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1725,17 +1723,17 @@
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H38" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1744,17 +1742,17 @@
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28">
@@ -1763,26 +1761,26 @@
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E40" s="7"/>
       <c r="G40" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="28">
       <c r="A41" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>42</v>
@@ -1790,15 +1788,15 @@
       <c r="E41" s="30"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="17" customFormat="1" ht="28">
       <c r="A42" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
@@ -1811,27 +1809,27 @@
         <v>43</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="17" customFormat="1" ht="28">
       <c r="A43" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="G43" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1855,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1866,10 +1864,10 @@
         <v>4</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1877,10 +1875,10 @@
         <v>5</v>
       </c>
       <c r="G48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1888,10 +1886,10 @@
         <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H49" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1899,107 +1897,107 @@
         <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B51" s="15"/>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="15"/>
       <c r="G52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B53" s="15"/>
       <c r="G53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B54" s="15"/>
       <c r="G54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="15"/>
       <c r="G55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="15"/>
       <c r="G56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C27"/>
+    <mergeCell ref="D19:D27"/>
+    <mergeCell ref="E19:E27"/>
+    <mergeCell ref="A35:A36"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C27"/>
-    <mergeCell ref="D19:D27"/>
-    <mergeCell ref="E19:E27"/>
-    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updated states/substates spreadsheet with new DoorOpen screens, & updated change log
</commit_message>
<xml_diff>
--- a/docs/Ember states and sub-states.xlsx
+++ b/docs/Ember states and sub-states.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="400" windowWidth="17920" windowHeight="16060"/>
+    <workbookView xWindow="3120" yWindow="200" windowWidth="17920" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="116">
   <si>
     <t>State</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>maintenance (or ready, if Spark Printer Status was ready when the door was opened)</t>
+  </si>
+  <si>
+    <t>&lt;job name&gt; loaded. Shut door to start the print.</t>
   </si>
 </sst>
 </file>
@@ -504,8 +507,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -665,6 +678,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,26 +699,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -724,6 +737,11 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -754,6 +772,11 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1093,7 +1116,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1114,7 +1137,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="40"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1131,7 +1154,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="40"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="13" t="s">
         <v>61</v>
       </c>
@@ -1149,7 +1172,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="40"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
@@ -1166,7 +1189,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="13" t="s">
         <v>55</v>
       </c>
@@ -1183,7 +1206,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="28">
-      <c r="A7" s="40"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="13" t="s">
         <v>56</v>
       </c>
@@ -1204,7 +1227,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="40"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1225,7 +1248,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="40"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="13" t="s">
         <v>57</v>
       </c>
@@ -1244,7 +1267,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="13" t="s">
         <v>70</v>
       </c>
@@ -1263,7 +1286,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="40"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="13" t="s">
         <v>71</v>
       </c>
@@ -1282,7 +1305,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="40"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="13" t="s">
         <v>72</v>
       </c>
@@ -1301,7 +1324,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="13" t="s">
         <v>107</v>
       </c>
@@ -1322,7 +1345,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="28">
-      <c r="A14" s="41"/>
+      <c r="A14" s="45"/>
       <c r="B14" t="s">
         <v>108</v>
       </c>
@@ -1341,7 +1364,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="13"/>
@@ -1358,7 +1381,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="41"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="13" t="s">
         <v>91</v>
       </c>
@@ -1381,13 +1404,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="39" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="17" t="s">
@@ -1402,9 +1425,9 @@
         <v>111</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="47"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="40"/>
       <c r="G18" s="17" t="s">
         <v>82</v>
       </c>
@@ -1419,11 +1442,11 @@
       <c r="B19" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="G19" s="17" t="s">
         <v>79</v>
       </c>
@@ -1438,9 +1461,9 @@
       <c r="B20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="G20" s="17" t="s">
         <v>79</v>
       </c>
@@ -1455,9 +1478,9 @@
       <c r="B21" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
       <c r="G21" s="17" t="s">
         <v>79</v>
       </c>
@@ -1472,9 +1495,9 @@
       <c r="B22" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
       <c r="G22" s="17" t="s">
         <v>79</v>
       </c>
@@ -1489,9 +1512,9 @@
       <c r="B23" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="G23" s="17" t="s">
         <v>79</v>
       </c>
@@ -1506,9 +1529,9 @@
       <c r="B24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="G24" s="17" t="s">
         <v>79</v>
       </c>
@@ -1523,9 +1546,9 @@
       <c r="B25" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
       <c r="G25" s="17" t="s">
         <v>79</v>
       </c>
@@ -1540,9 +1563,9 @@
       <c r="B26" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
       <c r="G26" s="17" t="s">
         <v>79</v>
       </c>
@@ -1555,9 +1578,9 @@
         <v>66</v>
       </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
       <c r="G27" s="17" t="s">
         <v>79</v>
       </c>
@@ -1646,7 +1669,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="13"/>
@@ -1663,7 +1686,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="40"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="13" t="s">
         <v>16</v>
       </c>
@@ -1680,7 +1703,7 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="41"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="13" t="s">
         <v>19</v>
       </c>
@@ -1697,7 +1720,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="70">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="43" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="13"/>
@@ -1714,7 +1737,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="40"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="13" t="s">
         <v>21</v>
       </c>
@@ -1731,11 +1754,13 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="40"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="14"/>
+      <c r="C37" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="7"/>
       <c r="G37" s="17" t="s">
@@ -1746,11 +1771,13 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="40"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="14"/>
+      <c r="C38" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="D38" s="4"/>
       <c r="E38" s="7"/>
       <c r="G38" s="17" t="s">
@@ -1761,11 +1788,13 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="40"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="14"/>
+      <c r="C39" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D39" s="4"/>
       <c r="E39" s="7"/>
       <c r="G39" s="17" t="s">
@@ -1776,11 +1805,13 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="40"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="14"/>
+      <c r="C40" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="E40" s="7"/>
       <c r="G40" s="17" t="s">
@@ -1791,11 +1822,13 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="41"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="37"/>
+      <c r="C41" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="D41" s="4"/>
       <c r="E41" s="7"/>
       <c r="G41" s="17" t="s">
@@ -2095,16 +2128,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="C19:C27"/>
     <mergeCell ref="D19:D27"/>
     <mergeCell ref="E19:E27"/>
     <mergeCell ref="A35:A41"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updating doc for display of user name
</commit_message>
<xml_diff>
--- a/docs/Ember states and sub-states.xlsx
+++ b/docs/Ember states and sub-states.xlsx
@@ -137,9 +137,6 @@
     <t>Starting to print &lt;job name&gt;</t>
   </si>
   <si>
-    <t>Printing &lt;job name&gt;  &lt;hours:minutes&gt; remaining</t>
-  </si>
-  <si>
     <t>Cancel</t>
   </si>
   <si>
@@ -341,9 +338,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Was the print successful?</t>
-  </si>
-  <si>
     <t>DemoMode</t>
   </si>
   <si>
@@ -371,6 +365,12 @@
   </si>
   <si>
     <t xml:space="preserve">Error &lt;Ember error code&gt;:&lt;Linux errno&gt; &lt;short error message&gt; </t>
+  </si>
+  <si>
+    <t>Printing &lt;job name&gt;  &lt;hours:minutes&gt; remaining &lt;user name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;user name&gt; Was the print successful?</t>
   </si>
 </sst>
 </file>
@@ -649,25 +649,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>11</v>
@@ -1054,35 +1054,35 @@
         <v>2</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="38"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1092,51 +1092,51 @@
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
       <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" t="s">
         <v>80</v>
       </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="38"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="7"/>
       <c r="F4" s="16"/>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="38"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>64</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="38"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>36</v>
@@ -1144,16 +1144,16 @@
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28">
-      <c r="A7" s="38"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>31</v>
@@ -1165,14 +1165,14 @@
         <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="38"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
@@ -1186,16 +1186,16 @@
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="38"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>34</v>
@@ -1205,111 +1205,111 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="38"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="38"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="38"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="38"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>110</v>
-      </c>
       <c r="D13" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28">
-      <c r="A14" s="39"/>
+      <c r="A14" s="42"/>
       <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>111</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22" t="s">
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="13"/>
@@ -1319,29 +1319,29 @@
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="G15" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="39"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>93</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1349,54 +1349,54 @@
         <v>10</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="E17" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="40" t="s">
-        <v>40</v>
-      </c>
       <c r="G17" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="G18" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
       <c r="G19" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1404,101 +1404,101 @@
         <v>12</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
       <c r="G20" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="G21" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
       <c r="G22" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
       <c r="G23" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
       <c r="G24" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="G25" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1506,31 +1506,31 @@
         <v>8</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+        <v>64</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
       <c r="G26" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
       <c r="G27" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1539,36 +1539,36 @@
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="G28" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="7"/>
       <c r="G29" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1577,112 +1577,112 @@
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="G30" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="7"/>
       <c r="G32" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="38"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="7"/>
       <c r="G33" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="39"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="7"/>
       <c r="G34" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="41" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="7"/>
       <c r="G35" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="39"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="13" t="s">
         <v>21</v>
       </c>
@@ -1692,10 +1692,10 @@
       <c r="D36" s="4"/>
       <c r="E36" s="7"/>
       <c r="G36" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1704,17 +1704,17 @@
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="7"/>
       <c r="G37" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H37" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1723,17 +1723,17 @@
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H38" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1742,17 +1742,17 @@
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28">
@@ -1761,75 +1761,75 @@
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40" s="7"/>
       <c r="G40" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="28">
       <c r="A41" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E41" s="30"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="17" customFormat="1" ht="28">
       <c r="A42" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="22" t="s">
-        <v>43</v>
-      </c>
       <c r="G42" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="17" customFormat="1" ht="28">
       <c r="A43" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="G43" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1853,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1864,10 +1864,10 @@
         <v>4</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1875,10 +1875,10 @@
         <v>5</v>
       </c>
       <c r="G48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1886,10 +1886,10 @@
         <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H49" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1897,107 +1897,107 @@
         <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" s="15"/>
       <c r="G51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="15"/>
       <c r="G52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B53" s="15"/>
       <c r="G53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="15"/>
       <c r="G54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="15"/>
       <c r="G55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B56" s="15"/>
       <c r="G56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="C19:C27"/>
     <mergeCell ref="D19:D27"/>
     <mergeCell ref="E19:E27"/>
     <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
updating state machine diagram and states spreadsheet
</commit_message>
<xml_diff>
--- a/docs/Ember states and sub-states.xlsx
+++ b/docs/Ember states and sub-states.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="125">
   <si>
     <t>State</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>DoorOpen</t>
-  </si>
-  <si>
-    <t>ExitingDoorOpen</t>
   </si>
   <si>
     <t>&lt;clears previous screen&gt;</t>
@@ -371,6 +368,39 @@
   </si>
   <si>
     <t>&lt;user name&gt; Was the print successful?</t>
+  </si>
+  <si>
+    <t>ClearingScreen</t>
+  </si>
+  <si>
+    <t>ConfirmUpgrade</t>
+  </si>
+  <si>
+    <t>UpgradingProjector</t>
+  </si>
+  <si>
+    <t>UpgradeComplete</t>
+  </si>
+  <si>
+    <t>Upgrade projector*</t>
+  </si>
+  <si>
+    <t>*Projector upgrade option only provided if there's an I2C connection to the projector and it's not already running the latest projector firmware.</t>
+  </si>
+  <si>
+    <t>Want to upgrade the projector? EMBER MUST STAY POWERED</t>
+  </si>
+  <si>
+    <t>No, cancel</t>
+  </si>
+  <si>
+    <t>Yes, upgrade</t>
+  </si>
+  <si>
+    <t>Projector upgrade complete! Cycle Ember power to continue.</t>
+  </si>
+  <si>
+    <t>Projector upgrade in progress… KEEP EMBER POWERED UP</t>
   </si>
 </sst>
 </file>
@@ -504,7 +534,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -554,8 +584,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -649,6 +681,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,17 +705,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -696,6 +731,7 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -720,6 +756,7 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1019,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1030,7 +1067,7 @@
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="49.5" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="9" customWidth="1"/>
     <col min="6" max="6" width="2.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
@@ -1042,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>11</v>
@@ -1054,294 +1091,294 @@
         <v>2</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="43"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
       <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="43"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="7"/>
       <c r="F4" s="16"/>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="43"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="43"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
       <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28">
+      <c r="A7" s="39"/>
+      <c r="B7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
         <v>78</v>
       </c>
-      <c r="H6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28">
-      <c r="A7" s="43"/>
-      <c r="B7" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>79</v>
-      </c>
       <c r="H7" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="43"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="43"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="43"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="43"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="43"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="43"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28">
+      <c r="A14" s="40"/>
+      <c r="B14" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28">
-      <c r="A14" s="42"/>
-      <c r="B14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>109</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="G15" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="42"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>92</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1349,54 +1386,54 @@
         <v>10</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="37" t="s">
+      <c r="C17" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="37" t="s">
-        <v>39</v>
-      </c>
       <c r="G17" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="G18" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
       <c r="G19" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1404,101 +1441,101 @@
         <v>12</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
       <c r="G20" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
       <c r="G21" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
       <c r="G22" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
       <c r="G23" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
       <c r="G24" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
       <c r="G25" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1506,31 +1543,31 @@
         <v>8</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
       <c r="G26" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
       <c r="G27" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1539,36 +1576,36 @@
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="G28" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="7"/>
       <c r="G29" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1577,427 +1614,506 @@
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="G30" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="7"/>
       <c r="G32" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="43"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="39"/>
       <c r="B33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="7"/>
       <c r="G33" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="42"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="40"/>
       <c r="B34" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="7"/>
       <c r="G34" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="28">
-      <c r="A35" s="41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28">
+      <c r="A35" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="7"/>
       <c r="G35" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="42"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="40"/>
       <c r="B36" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>22</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="7"/>
       <c r="G36" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="7"/>
       <c r="G37" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H37" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="E38" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H38" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>84</v>
+      </c>
+      <c r="I38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28">
       <c r="A40" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E40" s="7"/>
       <c r="G40" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="28">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="28">
       <c r="A41" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41" s="30"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="17" customFormat="1" ht="28">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A42" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D42" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E42" s="22" t="s">
-        <v>42</v>
-      </c>
       <c r="G42" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="17" customFormat="1" ht="28">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="17" customFormat="1" ht="28">
       <c r="A43" s="35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="G43" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="8"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="17" customFormat="1">
+      <c r="A44" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="17" customFormat="1">
+      <c r="A45" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="21"/>
+      <c r="E45" s="22"/>
+      <c r="G45" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="17" customFormat="1">
+      <c r="A46" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="21"/>
+      <c r="E46" s="22"/>
+      <c r="G46" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="17" customFormat="1">
+      <c r="A47" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="22"/>
+      <c r="G47" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="8"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
-        <v>4</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" t="s">
-        <v>79</v>
-      </c>
-      <c r="H48" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" t="s">
-        <v>78</v>
-      </c>
-      <c r="H49" s="24" t="s">
-        <v>88</v>
-      </c>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H53" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
         <v>8</v>
       </c>
-      <c r="G50" t="s">
-        <v>81</v>
-      </c>
-      <c r="H50" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="15"/>
-      <c r="G51" t="s">
-        <v>81</v>
-      </c>
-      <c r="H51" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" s="15"/>
-      <c r="G52" t="s">
-        <v>81</v>
-      </c>
-      <c r="H52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="15"/>
-      <c r="G53" t="s">
-        <v>81</v>
-      </c>
-      <c r="H53" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="15"/>
       <c r="G54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="17" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B55" s="15"/>
       <c r="G55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B56" s="15"/>
       <c r="G56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="17" t="s">
-        <v>101</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B57" s="15"/>
       <c r="G57" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H57" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="G58" t="s">
+        <v>80</v>
+      </c>
+      <c r="H58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="G59" t="s">
+        <v>80</v>
+      </c>
+      <c r="H59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="15"/>
+      <c r="G60" t="s">
+        <v>80</v>
+      </c>
+      <c r="H60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" t="s">
+        <v>77</v>
+      </c>
+      <c r="H61" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C27"/>
+    <mergeCell ref="D19:D27"/>
+    <mergeCell ref="E19:E27"/>
+    <mergeCell ref="A35:A36"/>
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C27"/>
-    <mergeCell ref="D19:D27"/>
-    <mergeCell ref="E19:E27"/>
-    <mergeCell ref="A35:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>